<commit_message>
Changed M7 diode in BoM.
</commit_message>
<xml_diff>
--- a/cam/Leo_v1.0_2021-05-24-BoM.xlsx
+++ b/cam/Leo_v1.0_2021-05-24-BoM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\LEO-32U4\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A06A728-2BD6-4BE3-B9CF-3B93057087FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E77BB4-4D37-482B-ABBE-EF42ACA08F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24130" yWindow="780" windowWidth="16430" windowHeight="19950" xr2:uid="{E4FE3D67-306B-4284-A7EC-952F0BAEDD36}"/>
+    <workbookView xWindow="23340" yWindow="990" windowWidth="17320" windowHeight="19950" xr2:uid="{E4FE3D67-306B-4284-A7EC-952F0BAEDD36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -260,9 +260,6 @@
     <t>C15849</t>
   </si>
   <si>
-    <t>C366566</t>
-  </si>
-  <si>
     <t>C151168</t>
   </si>
   <si>
@@ -336,6 +333,9 @@
   </si>
   <si>
     <t>C44854</t>
+  </si>
+  <si>
+    <t>C95872</t>
   </si>
 </sst>
 </file>
@@ -402,13 +402,13 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -482,11 +482,11 @@
   </sortState>
   <tableColumns count="6">
     <tableColumn id="35" xr3:uid="{E4D6D7C9-59A7-4DF3-86AD-FB15217418D5}" uniqueName="35" name="Qty" queryTableFieldId="1"/>
-    <tableColumn id="37" xr3:uid="{3D5D46C9-4611-4A74-9F05-4DC0B142819C}" uniqueName="37" name="Designator" queryTableFieldId="36" dataDxfId="2"/>
-    <tableColumn id="38" xr3:uid="{9ADE2975-0145-409D-A39B-DB5DF2F8F732}" uniqueName="38" name="Footprint" queryTableFieldId="37" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{80A4D8C9-48BE-4630-B8B2-A5B6EB1B17F7}" uniqueName="2" name="Comment" queryTableFieldId="2" dataDxfId="4"/>
-    <tableColumn id="40" xr3:uid="{05CEE9A9-B7A4-4608-A5DC-8B76BB69BE21}" uniqueName="40" name="LCSC Part #" queryTableFieldId="38" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{2395B02D-CBB8-40C4-8E60-4D6BCF5A6A3C}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="3"/>
+    <tableColumn id="37" xr3:uid="{3D5D46C9-4611-4A74-9F05-4DC0B142819C}" uniqueName="37" name="Designator" queryTableFieldId="36" dataDxfId="4"/>
+    <tableColumn id="38" xr3:uid="{9ADE2975-0145-409D-A39B-DB5DF2F8F732}" uniqueName="38" name="Footprint" queryTableFieldId="37" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{80A4D8C9-48BE-4630-B8B2-A5B6EB1B17F7}" uniqueName="2" name="Comment" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="40" xr3:uid="{05CEE9A9-B7A4-4608-A5DC-8B76BB69BE21}" uniqueName="40" name="LCSC Part #" queryTableFieldId="38" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{2395B02D-CBB8-40C4-8E60-4D6BCF5A6A3C}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -792,7 +792,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -939,8 +939,8 @@
       <c r="D7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>74</v>
+      <c r="E7" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>58</v>
@@ -960,7 +960,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>20</v>
@@ -974,13 +974,13 @@
         <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>36</v>
@@ -994,13 +994,13 @@
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>36</v>
@@ -1014,13 +1014,13 @@
         <v>53</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>54</v>
@@ -1040,7 +1040,7 @@
         <v>50</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>52</v>
@@ -1054,13 +1054,13 @@
         <v>49</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>47</v>
@@ -1074,13 +1074,13 @@
         <v>46</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>45</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>47</v>
@@ -1094,13 +1094,13 @@
         <v>60</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>47</v>
@@ -1114,13 +1114,13 @@
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>16</v>
@@ -1140,7 +1140,7 @@
         <v>27</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>4</v>
@@ -1160,7 +1160,7 @@
         <v>8</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>4</v>
@@ -1180,7 +1180,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>4</v>
@@ -1200,7 +1200,7 @@
         <v>23</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>4</v>
@@ -1220,7 +1220,7 @@
         <v>21</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>4</v>
@@ -1234,13 +1234,13 @@
         <v>40</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>41</v>
@@ -1254,13 +1254,13 @@
         <v>30</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>31</v>
@@ -1274,13 +1274,13 @@
         <v>43</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>44</v>
@@ -1293,27 +1293,26 @@
     <hyperlink ref="E4" r:id="rId2" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL21A106KAYNNNE_10uF-106-10-25V_C15850.html/?href=jlc-SMT" xr:uid="{2D22417F-92EE-4AD0-B9C8-E1CBDEC040FF}"/>
     <hyperlink ref="E3" r:id="rId3" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_12pF-120-5-50V_C1547.html/?href=jlc-SMT" xr:uid="{485420E0-AE49-46CD-B8F5-A3A1B5E6B862}"/>
     <hyperlink ref="E5" r:id="rId4" display="https://lcsc.com/product-detail/Multilayer-Ceramic-Capacitors-MLCC-SMD-SMT_SAMSUNG_CL05B104KO5NNNC_100nF-104-10-16V_C1525.html/?href=jlc-SMT" xr:uid="{6D8F993F-FD64-4104-A723-F8463FA66B28}"/>
-    <hyperlink ref="E7" r:id="rId5" display="https://lcsc.com/product-detail/Others_DOWO-M7_C366566.html/?href=jlc-SMT" xr:uid="{06E2EF48-6CA8-4DE9-8B26-A27E1C331E82}"/>
-    <hyperlink ref="E8" r:id="rId6" display="https://lcsc.com/product-detail/PTC-Resettable-Fuses_Littelfuse-1812L050-30PR_C151168.html/?href=jlc-SMT" xr:uid="{02B4CC6A-4D9D-4BE6-A373-D893C4548945}"/>
-    <hyperlink ref="E10" r:id="rId7" display="https://lcsc.com/product-detail/Low-Dropout-Regulators-LDO_AMS_AMS1117-3-3_AMS1117-3-3_C6186.html/?href=jlc-SMT" xr:uid="{7F8DA255-BD7F-495E-B7E2-53C05FDED67B}"/>
-    <hyperlink ref="E9" r:id="rId8" display="https://lcsc.com/product-detail/Low-Dropout-Regulators-LDO_AMS_AMS1117-5-0_AMS1117-5-0_C6187.html/?href=jlc-SMT" xr:uid="{1C55F031-2FCD-44D2-8C7C-7EB7A2989C34}"/>
-    <hyperlink ref="E11" r:id="rId9" display="https://lcsc.com/product-detail/General-Purpose-Amplifiers_ON-Semicon_LM358DR2G_ON-Semicon-ON-LM358DR2G_C7950.html/?href=jlc-SMT" xr:uid="{B9739C41-2C00-45AC-A4AC-1E1C36043E01}"/>
-    <hyperlink ref="E12" r:id="rId10" display="https://lcsc.com/product-detail/Beads_Sunlord-GZ2012D601TF_C1017.html/?href=jlc-SMT" xr:uid="{9F9D5563-0954-4DE1-A87F-FE14C876016C}"/>
-    <hyperlink ref="E14" r:id="rId11" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_0603-Blue-light_C72041.html/?href=jlc-SMT" xr:uid="{80E9A66E-AE09-4026-8425-F8CAA3EE0846}"/>
-    <hyperlink ref="E13" r:id="rId12" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_0603-Green-light_C72043.html/?href=jlc-SMT" xr:uid="{5C31F926-F3D3-4960-958B-29F22286F506}"/>
-    <hyperlink ref="E15" r:id="rId13" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_0603-Yellow-light_C72038.html/?href=jlc-SMT" xr:uid="{F760EA54-ED35-43F4-AEF9-A9FD5351CF46}"/>
-    <hyperlink ref="E16" r:id="rId14" display="https://lcsc.com/product-detail/SMD-Crystal-Resonators_Yangxing-Tech-X322516MLB4SI_C13738.html/?href=jlc-SMT" xr:uid="{34C5CE0F-025B-4A82-A63D-80E3E89E067B}"/>
-    <hyperlink ref="E17" r:id="rId15" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{1FE28CE6-FBEC-4C72-8C6A-C0A34B6B5374}"/>
-    <hyperlink ref="E18" r:id="rId16" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF1002TCE_C25744.html/?href=jlc-SMT" xr:uid="{66C71394-35C2-4D6D-BF77-0BAE8FD646CB}"/>
-    <hyperlink ref="E19" r:id="rId17" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF1003TCE_C25741.html/?href=jlc-SMT" xr:uid="{7579A862-8B46-4F63-9EDB-17E636BB1B5C}"/>
-    <hyperlink ref="E20" r:id="rId18" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF1004TCE_C26083.html/?href=jlc-SMT" xr:uid="{568D2596-BD39-4144-A7A8-4509DB953707}"/>
-    <hyperlink ref="E21" r:id="rId19" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF1001TCE_C11702.html/?href=jlc-SMT" xr:uid="{CF3E36B6-3D99-40E8-941F-7188CFF3E838}"/>
-    <hyperlink ref="E23" r:id="rId20" display="https://lcsc.com/product-detail/MOSFET_Changjiang-Electronics-Tech-CJ-2N7002_C8545.html/?href=jlc-SMT" xr:uid="{7182F06F-8F4A-4D56-B5B1-47686BB7BB3E}"/>
+    <hyperlink ref="E8" r:id="rId5" display="https://lcsc.com/product-detail/PTC-Resettable-Fuses_Littelfuse-1812L050-30PR_C151168.html/?href=jlc-SMT" xr:uid="{02B4CC6A-4D9D-4BE6-A373-D893C4548945}"/>
+    <hyperlink ref="E10" r:id="rId6" display="https://lcsc.com/product-detail/Low-Dropout-Regulators-LDO_AMS_AMS1117-3-3_AMS1117-3-3_C6186.html/?href=jlc-SMT" xr:uid="{7F8DA255-BD7F-495E-B7E2-53C05FDED67B}"/>
+    <hyperlink ref="E9" r:id="rId7" display="https://lcsc.com/product-detail/Low-Dropout-Regulators-LDO_AMS_AMS1117-5-0_AMS1117-5-0_C6187.html/?href=jlc-SMT" xr:uid="{1C55F031-2FCD-44D2-8C7C-7EB7A2989C34}"/>
+    <hyperlink ref="E11" r:id="rId8" display="https://lcsc.com/product-detail/General-Purpose-Amplifiers_ON-Semicon_LM358DR2G_ON-Semicon-ON-LM358DR2G_C7950.html/?href=jlc-SMT" xr:uid="{B9739C41-2C00-45AC-A4AC-1E1C36043E01}"/>
+    <hyperlink ref="E12" r:id="rId9" display="https://lcsc.com/product-detail/Beads_Sunlord-GZ2012D601TF_C1017.html/?href=jlc-SMT" xr:uid="{9F9D5563-0954-4DE1-A87F-FE14C876016C}"/>
+    <hyperlink ref="E14" r:id="rId10" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_0603-Blue-light_C72041.html/?href=jlc-SMT" xr:uid="{80E9A66E-AE09-4026-8425-F8CAA3EE0846}"/>
+    <hyperlink ref="E13" r:id="rId11" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_0603-Green-light_C72043.html/?href=jlc-SMT" xr:uid="{5C31F926-F3D3-4960-958B-29F22286F506}"/>
+    <hyperlink ref="E15" r:id="rId12" display="https://lcsc.com/product-detail/Light-Emitting-Diodes-LED_0603-Yellow-light_C72038.html/?href=jlc-SMT" xr:uid="{F760EA54-ED35-43F4-AEF9-A9FD5351CF46}"/>
+    <hyperlink ref="E16" r:id="rId13" display="https://lcsc.com/product-detail/SMD-Crystal-Resonators_Yangxing-Tech-X322516MLB4SI_C13738.html/?href=jlc-SMT" xr:uid="{34C5CE0F-025B-4A82-A63D-80E3E89E067B}"/>
+    <hyperlink ref="E17" r:id="rId14" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF220JTCE_C25092.html/?href=jlc-SMT" xr:uid="{1FE28CE6-FBEC-4C72-8C6A-C0A34B6B5374}"/>
+    <hyperlink ref="E18" r:id="rId15" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF1002TCE_C25744.html/?href=jlc-SMT" xr:uid="{66C71394-35C2-4D6D-BF77-0BAE8FD646CB}"/>
+    <hyperlink ref="E19" r:id="rId16" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF1003TCE_C25741.html/?href=jlc-SMT" xr:uid="{7579A862-8B46-4F63-9EDB-17E636BB1B5C}"/>
+    <hyperlink ref="E20" r:id="rId17" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF1004TCE_C26083.html/?href=jlc-SMT" xr:uid="{568D2596-BD39-4144-A7A8-4509DB953707}"/>
+    <hyperlink ref="E21" r:id="rId18" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_Uniroyal-Elec-0402WGF1001TCE_C11702.html/?href=jlc-SMT" xr:uid="{CF3E36B6-3D99-40E8-941F-7188CFF3E838}"/>
+    <hyperlink ref="E23" r:id="rId19" display="https://lcsc.com/product-detail/MOSFET_Changjiang-Electronics-Tech-CJ-2N7002_C8545.html/?href=jlc-SMT" xr:uid="{7182F06F-8F4A-4D56-B5B1-47686BB7BB3E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId21"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId20"/>
   <tableParts count="1">
-    <tablePart r:id="rId22"/>
+    <tablePart r:id="rId21"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>